<commit_message>
Se cambia la extension a jpg
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeharo\Documents\dev\tarot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPMENT\dev\tarot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4638EA-8AF3-4D98-B784-6A1483C1DFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99803482-CE5F-4DBA-91DB-23431B65B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1260" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -587,24 +587,24 @@
         <v>40</v>
       </c>
       <c r="G1" t="str">
-        <f>CONCATENATE("'",A1,".png","',")</f>
-        <v>'0B.png',</v>
+        <f>CONCATENATE("'",A1,".jpg","',")</f>
+        <v>'0B.jpg',</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:K16" si="0">CONCATENATE("'",B1,".png","',")</f>
-        <v>'0E.png',</v>
+        <f t="shared" ref="H1:K16" si="0">CONCATENATE("'",B1,".jpg","',")</f>
+        <v>'0E.jpg',</v>
       </c>
       <c r="I1" t="str">
         <f t="shared" si="0"/>
-        <v>'0O.png',</v>
+        <v>'0O.jpg',</v>
       </c>
       <c r="J1" t="str">
         <f t="shared" si="0"/>
-        <v>'0C.png',</v>
+        <v>'0C.jpg',</v>
       </c>
       <c r="K1" t="str">
         <f t="shared" si="0"/>
-        <v>'0X.png',</v>
+        <v>'0X.jpg',</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -624,24 +624,24 @@
         <v>41</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G11" si="1">CONCATENATE("'",A2,".png","',")</f>
-        <v>'1B.png',</v>
+        <f t="shared" ref="G2:G22" si="1">CONCATENATE("'",A2,".jpg","',")</f>
+        <v>'1B.jpg',</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" si="0"/>
-        <v>'1E.png',</v>
+        <v>'1E.jpg',</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" si="0"/>
-        <v>'1O.png',</v>
+        <v>'1O.jpg',</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" si="0"/>
-        <v>'1C.png',</v>
+        <v>'1C.jpg',</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" si="0"/>
-        <v>'1X.png',</v>
+        <v>'1X.jpg',</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -662,23 +662,23 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="1"/>
-        <v>'2B.png',</v>
+        <v>'2B.jpg',</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
-        <v>'2E.png',</v>
+        <v>'2E.jpg',</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
-        <v>'2O.png',</v>
+        <v>'2O.jpg',</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>'2C.png',</v>
+        <v>'2C.jpg',</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
-        <v>'2X.png',</v>
+        <v>'2X.jpg',</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -699,23 +699,23 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
-        <v>'3B.png',</v>
+        <v>'3B.jpg',</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>'3E.png',</v>
+        <v>'3E.jpg',</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>'3O.png',</v>
+        <v>'3O.jpg',</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>'3C.png',</v>
+        <v>'3C.jpg',</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
-        <v>'3X.png',</v>
+        <v>'3X.jpg',</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -736,23 +736,23 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
-        <v>'4B.png',</v>
+        <v>'4B.jpg',</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>'4E.png',</v>
+        <v>'4E.jpg',</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>'4O.png',</v>
+        <v>'4O.jpg',</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>'4C.png',</v>
+        <v>'4C.jpg',</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
-        <v>'4X.png',</v>
+        <v>'4X.jpg',</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -773,23 +773,23 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
-        <v>'5B.png',</v>
+        <v>'5B.jpg',</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>'5E.png',</v>
+        <v>'5E.jpg',</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>'5O.png',</v>
+        <v>'5O.jpg',</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>'5C.png',</v>
+        <v>'5C.jpg',</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>'5X.png',</v>
+        <v>'5X.jpg',</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -810,23 +810,23 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>'6B.png',</v>
+        <v>'6B.jpg',</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>'6E.png',</v>
+        <v>'6E.jpg',</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>'6O.png',</v>
+        <v>'6O.jpg',</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>'6C.png',</v>
+        <v>'6C.jpg',</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>'6X.png',</v>
+        <v>'6X.jpg',</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -847,23 +847,23 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>'7B.png',</v>
+        <v>'7B.jpg',</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>'7E.png',</v>
+        <v>'7E.jpg',</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>'7O.png',</v>
+        <v>'7O.jpg',</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>'7C.png',</v>
+        <v>'7C.jpg',</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>'7X.png',</v>
+        <v>'7X.jpg',</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -884,23 +884,23 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
-        <v>'8B.png',</v>
+        <v>'8B.jpg',</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>'8E.png',</v>
+        <v>'8E.jpg',</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>'8O.png',</v>
+        <v>'8O.jpg',</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>'8C.png',</v>
+        <v>'8C.jpg',</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>'8X.png',</v>
+        <v>'8X.jpg',</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -921,23 +921,23 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>'9B.png',</v>
+        <v>'9B.jpg',</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>'9E.png',</v>
+        <v>'9E.jpg',</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>'9O.png',</v>
+        <v>'9O.jpg',</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>'9C.png',</v>
+        <v>'9C.jpg',</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>'9X.png',</v>
+        <v>'9X.jpg',</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -958,23 +958,23 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
-        <v>'10B.png',</v>
+        <v>'10B.jpg',</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>'10E.png',</v>
+        <v>'10E.jpg',</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>'10O.png',</v>
+        <v>'10O.jpg',</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>'10C.png',</v>
+        <v>'10C.jpg',</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>'10X.png',</v>
+        <v>'10X.jpg',</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -994,24 +994,24 @@
         <v>51</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" ref="G12" si="2">CONCATENATE("'",A12,".png","',")</f>
-        <v>'11B.png',</v>
+        <f t="shared" si="1"/>
+        <v>'11B.jpg',</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" ref="H12" si="3">CONCATENATE("'",B12,".png","',")</f>
-        <v>'11E.png',</v>
+        <f t="shared" si="0"/>
+        <v>'11E.jpg',</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12" si="4">CONCATENATE("'",C12,".png","',")</f>
-        <v>'11O.png',</v>
+        <f t="shared" si="0"/>
+        <v>'11O.jpg',</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12" si="5">CONCATENATE("'",D12,".png","',")</f>
-        <v>'11C.png',</v>
+        <f t="shared" si="0"/>
+        <v>'11C.jpg',</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>'11X.png',</v>
+        <v>'11X.jpg',</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>'12X.png',</v>
+        <v>'12X.jpg',</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>'13X.png',</v>
+        <v>'13X.jpg',</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>'14X.png',</v>
+        <v>'14X.jpg',</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>'15X.png',</v>
+        <v>'15X.jpg',</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
@@ -1055,8 +1055,8 @@
         <v>56</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:K22" si="6">CONCATENATE("'",E17,".png","',")</f>
-        <v>'16X.png',</v>
+        <f t="shared" ref="K17:K22" si="2">CONCATENATE("'",E17,".jpg","',")</f>
+        <v>'16X.jpg',</v>
       </c>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
@@ -1064,8 +1064,8 @@
         <v>57</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="6"/>
-        <v>'17X.png',</v>
+        <f t="shared" si="2"/>
+        <v>'17X.jpg',</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
@@ -1073,8 +1073,8 @@
         <v>58</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="6"/>
-        <v>'18X.png',</v>
+        <f t="shared" si="2"/>
+        <v>'18X.jpg',</v>
       </c>
     </row>
     <row r="20" spans="5:11" x14ac:dyDescent="0.25">
@@ -1082,8 +1082,8 @@
         <v>59</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="6"/>
-        <v>'19X.png',</v>
+        <f t="shared" si="2"/>
+        <v>'19X.jpg',</v>
       </c>
     </row>
     <row r="21" spans="5:11" x14ac:dyDescent="0.25">
@@ -1091,8 +1091,8 @@
         <v>60</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="6"/>
-        <v>'20X.png',</v>
+        <f t="shared" si="2"/>
+        <v>'20X.jpg',</v>
       </c>
     </row>
     <row r="22" spans="5:11" x14ac:dyDescent="0.25">
@@ -1100,8 +1100,8 @@
         <v>61</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="6"/>
-        <v>'21X.png',</v>
+        <f t="shared" si="2"/>
+        <v>'21X.jpg',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añade tarot de riderwaite y boton de seleccion de tipo de baraja
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPMENT\dev\tarot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99803482-CE5F-4DBA-91DB-23431B65B967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE36606B-5A74-4AF5-B0EB-1907C69D8D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
-  <si>
-    <t>0B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>1B</t>
   </si>
@@ -67,9 +64,6 @@
     <t>6B</t>
   </si>
   <si>
-    <t>0E</t>
-  </si>
-  <si>
     <t>1E</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>9E</t>
   </si>
   <si>
-    <t>0O</t>
-  </si>
-  <si>
     <t>1O</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>9O</t>
   </si>
   <si>
-    <t>0C</t>
-  </si>
-  <si>
     <t>1C</t>
   </si>
   <si>
@@ -245,16 +233,58 @@
   </si>
   <si>
     <t>11C</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>13B</t>
+  </si>
+  <si>
+    <t>14B</t>
+  </si>
+  <si>
+    <t>12E</t>
+  </si>
+  <si>
+    <t>14E</t>
+  </si>
+  <si>
+    <t>13E</t>
+  </si>
+  <si>
+    <t>12O</t>
+  </si>
+  <si>
+    <t>13O</t>
+  </si>
+  <si>
+    <t>14O</t>
+  </si>
+  <si>
+    <t>12C</t>
+  </si>
+  <si>
+    <t>13C</t>
+  </si>
+  <si>
+    <t>14C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,7 +595,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="G1:K22"/>
+      <selection activeCell="G1" sqref="G1:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,35 +605,35 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G1" t="str">
         <f>CONCATENATE("'",A1,".jpg","',")</f>
-        <v>'0B.jpg',</v>
+        <v>'1B.jpg',</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:K16" si="0">CONCATENATE("'",B1,".jpg","',")</f>
-        <v>'0E.jpg',</v>
+        <f>CONCATENATE("'",B1,".jpg","',")</f>
+        <v>'1E.jpg',</v>
       </c>
       <c r="I1" t="str">
-        <f t="shared" si="0"/>
-        <v>'0O.jpg',</v>
+        <f>CONCATENATE("'",C1,".jpg","',")</f>
+        <v>'1O.jpg',</v>
       </c>
       <c r="J1" t="str">
-        <f t="shared" si="0"/>
-        <v>'0C.jpg',</v>
+        <f>CONCATENATE("'",D1,".jpg","',")</f>
+        <v>'1C.jpg',</v>
       </c>
       <c r="K1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K1" si="0">CONCATENATE("'",E1,".jpg","',")</f>
         <v>'0X.jpg',</v>
       </c>
     </row>
@@ -612,35 +642,35 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G22" si="1">CONCATENATE("'",A2,".jpg","',")</f>
-        <v>'1B.jpg',</v>
+        <f>CONCATENATE("'",A2,".jpg","',")</f>
+        <v>'2B.jpg',</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" si="0"/>
-        <v>'1E.jpg',</v>
+        <f>CONCATENATE("'",B2,".jpg","',")</f>
+        <v>'2E.jpg',</v>
       </c>
       <c r="I2" t="str">
-        <f t="shared" si="0"/>
-        <v>'1O.jpg',</v>
+        <f>CONCATENATE("'",C2,".jpg","',")</f>
+        <v>'2O.jpg',</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" si="0"/>
-        <v>'1C.jpg',</v>
+        <f>CONCATENATE("'",D2,".jpg","',")</f>
+        <v>'2C.jpg',</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H1:K16" si="1">CONCATENATE("'",E2,".jpg","',")</f>
         <v>'1X.jpg',</v>
       </c>
     </row>
@@ -649,35 +679,35 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="1"/>
-        <v>'2B.jpg',</v>
+        <f>CONCATENATE("'",A3,".jpg","',")</f>
+        <v>'3B.jpg',</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" si="0"/>
-        <v>'2E.jpg',</v>
+        <f>CONCATENATE("'",B3,".jpg","',")</f>
+        <v>'3E.jpg',</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>'2O.jpg',</v>
+        <f>CONCATENATE("'",C3,".jpg","',")</f>
+        <v>'3O.jpg',</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" si="0"/>
-        <v>'2C.jpg',</v>
+        <f>CONCATENATE("'",D3,".jpg","',")</f>
+        <v>'3C.jpg',</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'2X.jpg',</v>
       </c>
     </row>
@@ -686,35 +716,35 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="1"/>
-        <v>'3B.jpg',</v>
+        <f>CONCATENATE("'",A4,".jpg","',")</f>
+        <v>'4B.jpg',</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>'3E.jpg',</v>
+        <f>CONCATENATE("'",B4,".jpg","',")</f>
+        <v>'4E.jpg',</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>'3O.jpg',</v>
+        <f>CONCATENATE("'",C4,".jpg","',")</f>
+        <v>'4O.jpg',</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>'3C.jpg',</v>
+        <f>CONCATENATE("'",D4,".jpg","',")</f>
+        <v>'4C.jpg',</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'3X.jpg',</v>
       </c>
     </row>
@@ -723,109 +753,109 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="1"/>
-        <v>'4B.jpg',</v>
+        <f>CONCATENATE("'",A5,".jpg","',")</f>
+        <v>'5B.jpg',</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>'4E.jpg',</v>
+        <f>CONCATENATE("'",B5,".jpg","',")</f>
+        <v>'5E.jpg',</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>'4O.jpg',</v>
+        <f>CONCATENATE("'",C5,".jpg","',")</f>
+        <v>'5O.jpg',</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>'4C.jpg',</v>
+        <f>CONCATENATE("'",D5,".jpg","',")</f>
+        <v>'5C.jpg',</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'4X.jpg',</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="1"/>
-        <v>'5B.jpg',</v>
+        <f>CONCATENATE("'",A6,".jpg","',")</f>
+        <v>'6B.jpg',</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>'5E.jpg',</v>
+        <f>CONCATENATE("'",B6,".jpg","',")</f>
+        <v>'6E.jpg',</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>'5O.jpg',</v>
+        <f>CONCATENATE("'",C6,".jpg","',")</f>
+        <v>'6O.jpg',</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>'5C.jpg',</v>
+        <f>CONCATENATE("'",D6,".jpg","',")</f>
+        <v>'6C.jpg',</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'5X.jpg',</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
-        <v>'6B.jpg',</v>
+        <f>CONCATENATE("'",A7,".jpg","',")</f>
+        <v>'7B.jpg',</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>'6E.jpg',</v>
+        <f>CONCATENATE("'",B7,".jpg","',")</f>
+        <v>'7E.jpg',</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>'6O.jpg',</v>
+        <f>CONCATENATE("'",C7,".jpg","',")</f>
+        <v>'7O.jpg',</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>'6C.jpg',</v>
+        <f>CONCATENATE("'",D7,".jpg","',")</f>
+        <v>'7C.jpg',</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'6X.jpg',</v>
       </c>
     </row>
@@ -834,35 +864,35 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="1"/>
-        <v>'7B.jpg',</v>
+        <f>CONCATENATE("'",A8,".jpg","',")</f>
+        <v>'8B.jpg',</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>'7E.jpg',</v>
+        <f>CONCATENATE("'",B8,".jpg","',")</f>
+        <v>'8E.jpg',</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>'7O.jpg',</v>
+        <f>CONCATENATE("'",C8,".jpg","',")</f>
+        <v>'8O.jpg',</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>'7C.jpg',</v>
+        <f>CONCATENATE("'",D8,".jpg","',")</f>
+        <v>'8C.jpg',</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'7X.jpg',</v>
       </c>
     </row>
@@ -871,72 +901,72 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="1"/>
-        <v>'8B.jpg',</v>
+        <f>CONCATENATE("'",A9,".jpg","',")</f>
+        <v>'9B.jpg',</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>'8E.jpg',</v>
+        <f>CONCATENATE("'",B9,".jpg","',")</f>
+        <v>'9E.jpg',</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>'8O.jpg',</v>
+        <f>CONCATENATE("'",C9,".jpg","',")</f>
+        <v>'9O.jpg',</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>'8C.jpg',</v>
+        <f>CONCATENATE("'",D9,".jpg","',")</f>
+        <v>'9C.jpg',</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'8X.jpg',</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
-        <v>'9B.jpg',</v>
+        <f>CONCATENATE("'",A10,".jpg","',")</f>
+        <v>'10B.jpg',</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>'9E.jpg',</v>
+        <f>CONCATENATE("'",B10,".jpg","',")</f>
+        <v>'10E.jpg',</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>'9O.jpg',</v>
+        <f>CONCATENATE("'",C10,".jpg","',")</f>
+        <v>'10O.jpg',</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>'9C.jpg',</v>
+        <f>CONCATENATE("'",D10,".jpg","',")</f>
+        <v>'10C.jpg',</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'9X.jpg',</v>
       </c>
     </row>
@@ -954,26 +984,26 @@
         <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="1"/>
-        <v>'10B.jpg',</v>
+        <f>CONCATENATE("'",A12,".jpg","',")</f>
+        <v>'12B.jpg',</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>'10E.jpg',</v>
+        <f>CONCATENATE("'",B11,".jpg","',")</f>
+        <v>'11E.jpg',</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>'10O.jpg',</v>
+        <f>CONCATENATE("'",C11,".jpg","',")</f>
+        <v>'11O.jpg',</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>'10C.jpg',</v>
+        <f>CONCATENATE("'",D11,".jpg","',")</f>
+        <v>'11C.jpg',</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'10X.jpg',</v>
       </c>
     </row>
@@ -982,129 +1012,186 @@
         <v>66</v>
       </c>
       <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ref="G12:G14" si="2">CONCATENATE("'",A13,".jpg","',")</f>
+        <v>'13B.jpg',</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" ref="H12:H14" si="3">CONCATENATE("'",B12,".jpg","',")</f>
+        <v>'12E.jpg',</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ref="I12:I14" si="4">CONCATENATE("'",C12,".jpg","',")</f>
+        <v>'12O.jpg',</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ref="J12:J14" si="5">CONCATENATE("'",D12,".jpg","',")</f>
+        <v>'12C.jpg',</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>'11X.jpg',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>'14B.jpg',</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>'13E.jpg',</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="4"/>
+        <v>'13O.jpg',</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="5"/>
+        <v>'13C.jpg',</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>'12X.jpg',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>68</v>
       </c>
-      <c r="D12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G12" t="str">
-        <f t="shared" si="1"/>
-        <v>'11B.jpg',</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>'11E.jpg',</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>'11O.jpg',</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>'11C.jpg',</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="0"/>
-        <v>'11X.jpg',</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="0"/>
-        <v>'12X.jpg',</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>'.jpg',</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>'14E.jpg',</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="4"/>
+        <v>'14O.jpg',</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="5"/>
+        <v>'14C.jpg',</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'13X.jpg',</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'14X.jpg',</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'15X.jpg',</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:K22" si="2">CONCATENATE("'",E17,".jpg","',")</f>
+        <f t="shared" ref="K17:K22" si="6">CONCATENATE("'",E17,".jpg","',")</f>
         <v>'16X.jpg',</v>
       </c>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>'17X.jpg',</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>'18X.jpg',</v>
       </c>
     </row>
     <row r="20" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>'19X.jpg',</v>
       </c>
     </row>
     <row r="21" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>'20X.jpg',</v>
       </c>
     </row>
     <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>'21X.jpg',</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios con rose diversos
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEVELOPMENT\dev\tarot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE36606B-5A74-4AF5-B0EB-1907C69D8D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0774DC-C704-4B7C-9A06-BD4FC9C50F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,23 +617,23 @@
         <v>36</v>
       </c>
       <c r="G1" t="str">
-        <f>CONCATENATE("'",A1,".jpg","',")</f>
+        <f t="shared" ref="G1:G14" si="0">CONCATENATE("'",A1,".jpg","',")</f>
         <v>'1B.jpg',</v>
       </c>
       <c r="H1" t="str">
-        <f>CONCATENATE("'",B1,".jpg","',")</f>
+        <f t="shared" ref="H1:H10" si="1">CONCATENATE("'",B1,".jpg","',")</f>
         <v>'1E.jpg',</v>
       </c>
       <c r="I1" t="str">
-        <f>CONCATENATE("'",C1,".jpg","',")</f>
+        <f t="shared" ref="I1:I10" si="2">CONCATENATE("'",C1,".jpg","',")</f>
         <v>'1O.jpg',</v>
       </c>
       <c r="J1" t="str">
-        <f>CONCATENATE("'",D1,".jpg","',")</f>
+        <f t="shared" ref="J1:J10" si="3">CONCATENATE("'",D1,".jpg","',")</f>
         <v>'1C.jpg',</v>
       </c>
       <c r="K1" t="str">
-        <f t="shared" ref="K1" si="0">CONCATENATE("'",E1,".jpg","',")</f>
+        <f t="shared" ref="K1" si="4">CONCATENATE("'",E1,".jpg","',")</f>
         <v>'0X.jpg',</v>
       </c>
     </row>
@@ -654,23 +654,23 @@
         <v>37</v>
       </c>
       <c r="G2" t="str">
-        <f>CONCATENATE("'",A2,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'2B.jpg',</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE("'",B2,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'2E.jpg',</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("'",C2,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'2O.jpg',</v>
       </c>
       <c r="J2" t="str">
-        <f>CONCATENATE("'",D2,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'2C.jpg',</v>
       </c>
       <c r="K2" t="str">
-        <f t="shared" ref="H1:K16" si="1">CONCATENATE("'",E2,".jpg","',")</f>
+        <f t="shared" ref="K2:K16" si="5">CONCATENATE("'",E2,".jpg","',")</f>
         <v>'1X.jpg',</v>
       </c>
     </row>
@@ -691,23 +691,23 @@
         <v>38</v>
       </c>
       <c r="G3" t="str">
-        <f>CONCATENATE("'",A3,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'3B.jpg',</v>
       </c>
       <c r="H3" t="str">
-        <f>CONCATENATE("'",B3,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'3E.jpg',</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("'",C3,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'3O.jpg',</v>
       </c>
       <c r="J3" t="str">
-        <f>CONCATENATE("'",D3,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'3C.jpg',</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'2X.jpg',</v>
       </c>
     </row>
@@ -728,23 +728,23 @@
         <v>39</v>
       </c>
       <c r="G4" t="str">
-        <f>CONCATENATE("'",A4,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'4B.jpg',</v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE("'",B4,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'4E.jpg',</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE("'",C4,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'4O.jpg',</v>
       </c>
       <c r="J4" t="str">
-        <f>CONCATENATE("'",D4,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'4C.jpg',</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'3X.jpg',</v>
       </c>
     </row>
@@ -765,23 +765,23 @@
         <v>40</v>
       </c>
       <c r="G5" t="str">
-        <f>CONCATENATE("'",A5,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'5B.jpg',</v>
       </c>
       <c r="H5" t="str">
-        <f>CONCATENATE("'",B5,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'5E.jpg',</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE("'",C5,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'5O.jpg',</v>
       </c>
       <c r="J5" t="str">
-        <f>CONCATENATE("'",D5,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'5C.jpg',</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'4X.jpg',</v>
       </c>
     </row>
@@ -802,23 +802,23 @@
         <v>41</v>
       </c>
       <c r="G6" t="str">
-        <f>CONCATENATE("'",A6,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'6B.jpg',</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE("'",B6,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'6E.jpg',</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("'",C6,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'6O.jpg',</v>
       </c>
       <c r="J6" t="str">
-        <f>CONCATENATE("'",D6,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'6C.jpg',</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'5X.jpg',</v>
       </c>
     </row>
@@ -839,23 +839,23 @@
         <v>42</v>
       </c>
       <c r="G7" t="str">
-        <f>CONCATENATE("'",A7,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'7B.jpg',</v>
       </c>
       <c r="H7" t="str">
-        <f>CONCATENATE("'",B7,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'7E.jpg',</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("'",C7,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'7O.jpg',</v>
       </c>
       <c r="J7" t="str">
-        <f>CONCATENATE("'",D7,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'7C.jpg',</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'6X.jpg',</v>
       </c>
     </row>
@@ -876,23 +876,23 @@
         <v>43</v>
       </c>
       <c r="G8" t="str">
-        <f>CONCATENATE("'",A8,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'8B.jpg',</v>
       </c>
       <c r="H8" t="str">
-        <f>CONCATENATE("'",B8,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'8E.jpg',</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE("'",C8,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'8O.jpg',</v>
       </c>
       <c r="J8" t="str">
-        <f>CONCATENATE("'",D8,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'8C.jpg',</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'7X.jpg',</v>
       </c>
     </row>
@@ -913,23 +913,23 @@
         <v>44</v>
       </c>
       <c r="G9" t="str">
-        <f>CONCATENATE("'",A9,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'9B.jpg',</v>
       </c>
       <c r="H9" t="str">
-        <f>CONCATENATE("'",B9,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'9E.jpg',</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE("'",C9,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'9O.jpg',</v>
       </c>
       <c r="J9" t="str">
-        <f>CONCATENATE("'",D9,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'9C.jpg',</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'8X.jpg',</v>
       </c>
     </row>
@@ -950,23 +950,23 @@
         <v>45</v>
       </c>
       <c r="G10" t="str">
-        <f>CONCATENATE("'",A10,".jpg","',")</f>
+        <f t="shared" si="0"/>
         <v>'10B.jpg',</v>
       </c>
       <c r="H10" t="str">
-        <f>CONCATENATE("'",B10,".jpg","',")</f>
+        <f t="shared" si="1"/>
         <v>'10E.jpg',</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("'",C10,".jpg","',")</f>
+        <f t="shared" si="2"/>
         <v>'10O.jpg',</v>
       </c>
       <c r="J10" t="str">
-        <f>CONCATENATE("'",D10,".jpg","',")</f>
+        <f t="shared" si="3"/>
         <v>'10C.jpg',</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'9X.jpg',</v>
       </c>
     </row>
@@ -987,8 +987,8 @@
         <v>46</v>
       </c>
       <c r="G11" t="str">
-        <f>CONCATENATE("'",A12,".jpg","',")</f>
-        <v>'12B.jpg',</v>
+        <f t="shared" si="0"/>
+        <v>'11B.jpg',</v>
       </c>
       <c r="H11" t="str">
         <f>CONCATENATE("'",B11,".jpg","',")</f>
@@ -1003,7 +1003,7 @@
         <v>'11C.jpg',</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'10X.jpg',</v>
       </c>
     </row>
@@ -1024,23 +1024,23 @@
         <v>47</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" ref="G12:G14" si="2">CONCATENATE("'",A13,".jpg","',")</f>
-        <v>'13B.jpg',</v>
+        <f t="shared" si="0"/>
+        <v>'12B.jpg',</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" ref="H12:H14" si="3">CONCATENATE("'",B12,".jpg","',")</f>
+        <f t="shared" ref="H12:H14" si="6">CONCATENATE("'",B12,".jpg","',")</f>
         <v>'12E.jpg',</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12:I14" si="4">CONCATENATE("'",C12,".jpg","',")</f>
+        <f t="shared" ref="I12:I14" si="7">CONCATENATE("'",C12,".jpg","',")</f>
         <v>'12O.jpg',</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:J14" si="5">CONCATENATE("'",D12,".jpg","',")</f>
+        <f t="shared" ref="J12:J14" si="8">CONCATENATE("'",D12,".jpg","',")</f>
         <v>'12C.jpg',</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'11X.jpg',</v>
       </c>
     </row>
@@ -1061,23 +1061,23 @@
         <v>48</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="2"/>
-        <v>'14B.jpg',</v>
+        <f t="shared" si="0"/>
+        <v>'13B.jpg',</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>'13E.jpg',</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>'13O.jpg',</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>'13C.jpg',</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'12X.jpg',</v>
       </c>
     </row>
@@ -1098,23 +1098,23 @@
         <v>49</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="2"/>
-        <v>'.jpg',</v>
+        <f t="shared" si="0"/>
+        <v>'14B.jpg',</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>'14E.jpg',</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>'14O.jpg',</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>'14C.jpg',</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'13X.jpg',</v>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
         <v>50</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'14X.jpg',</v>
       </c>
     </row>
@@ -1132,7 +1132,7 @@
         <v>51</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>'15X.jpg',</v>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
         <v>52</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:K22" si="6">CONCATENATE("'",E17,".jpg","',")</f>
+        <f t="shared" ref="K17:K22" si="9">CONCATENATE("'",E17,".jpg","',")</f>
         <v>'16X.jpg',</v>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
         <v>53</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>'17X.jpg',</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
         <v>54</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>'18X.jpg',</v>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
         <v>55</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>'19X.jpg',</v>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
         <v>56</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>'20X.jpg',</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
         <v>57</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>'21X.jpg',</v>
       </c>
     </row>

</xml_diff>